<commit_message>
Added new test case for Negative login
</commit_message>
<xml_diff>
--- a/com.midcities.automation/TestData/Data.xlsx
+++ b/com.midcities.automation/TestData/Data.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Login_positive" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -28,19 +28,32 @@
   </si>
   <si>
     <t>Mcities12345</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,13 +73,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -359,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -383,7 +402,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added updated Test data excel file
</commit_message>
<xml_diff>
--- a/com.midcities.automation/TestData/Data.xlsx
+++ b/com.midcities.automation/TestData/Data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Admin_Features" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Username</t>
   </si>
@@ -34,13 +34,136 @@
   </si>
   <si>
     <t>test123</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Select permissions</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>testuser</t>
+  </si>
+  <si>
+    <t>testing90li@test.com</t>
+  </si>
+  <si>
+    <t>Add Customer</t>
+  </si>
+  <si>
+    <t>Add user</t>
+  </si>
+  <si>
+    <t>Business name</t>
+  </si>
+  <si>
+    <t>Point of contact</t>
+  </si>
+  <si>
+    <t>POC Phone</t>
+  </si>
+  <si>
+    <t>Business Phone</t>
+  </si>
+  <si>
+    <t>FAX number</t>
+  </si>
+  <si>
+    <t>Preferred mode of contact</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>test customer121</t>
+  </si>
+  <si>
+    <t>Test sample</t>
+  </si>
+  <si>
+    <t>test@test123.com</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>test same address</t>
+  </si>
+  <si>
+    <t>Customer notes</t>
+  </si>
+  <si>
+    <t>Test notes</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>98767890976</t>
+  </si>
+  <si>
+    <t>7687980965</t>
+  </si>
+  <si>
+    <t>Add Location</t>
+  </si>
+  <si>
+    <t>Location Type</t>
+  </si>
+  <si>
+    <t>Location name</t>
+  </si>
+  <si>
+    <t>Test Farm Rd  Wallace  North Carolina 28466  United States</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Hub</t>
+  </si>
+  <si>
+    <t>Test auto location</t>
+  </si>
+  <si>
+    <t>7656567567</t>
+  </si>
+  <si>
+    <t>Add Chassis</t>
+  </si>
+  <si>
+    <t>Chassis name</t>
+  </si>
+  <si>
+    <t>Test chassis company</t>
+  </si>
+  <si>
+    <t>test place</t>
+  </si>
+  <si>
+    <t>testchassis123@gmail.com</t>
+  </si>
+  <si>
+    <t>1432232322</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +177,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,9 +211,21 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -380,11 +523,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -420,13 +567,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="60">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C15" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new screens and changes
</commit_message>
<xml_diff>
--- a/com.midcities.automation/TestData/Data.xlsx
+++ b/com.midcities.automation/TestData/Data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin_Features" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Rate_Management" sheetId="3" r:id="rId3"/>
+    <sheet name="Order_Management" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="124">
   <si>
     <t>Username</t>
   </si>
@@ -157,6 +158,237 @@
   </si>
   <si>
     <t>1432232322</t>
+  </si>
+  <si>
+    <t>Add container</t>
+  </si>
+  <si>
+    <t>Container name</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>PCR</t>
+  </si>
+  <si>
+    <t>Hire/Dehire Location</t>
+  </si>
+  <si>
+    <t>Auto container</t>
+  </si>
+  <si>
+    <t>Chassis Depot Place</t>
+  </si>
+  <si>
+    <t>cont@testing.com</t>
+  </si>
+  <si>
+    <t>(222) 222-2222</t>
+  </si>
+  <si>
+    <t>bingTestLocation</t>
+  </si>
+  <si>
+    <t>NYU</t>
+  </si>
+  <si>
+    <t>Add equipment</t>
+  </si>
+  <si>
+    <t>Equipment type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>License state</t>
+  </si>
+  <si>
+    <t>License Expiry</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Dry</t>
+  </si>
+  <si>
+    <t>Test Equip</t>
+  </si>
+  <si>
+    <t>Test make</t>
+  </si>
+  <si>
+    <t>Test Model</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>Test license</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>1/1/2025</t>
+  </si>
+  <si>
+    <t>Central Lot KS</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Test Remarks</t>
+  </si>
+  <si>
+    <t>General route rate</t>
+  </si>
+  <si>
+    <t>Leg type</t>
+  </si>
+  <si>
+    <t>Driver Type</t>
+  </si>
+  <si>
+    <t>Rate Per Mile</t>
+  </si>
+  <si>
+    <t>Loaded</t>
+  </si>
+  <si>
+    <t>Companies</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Driver rates</t>
+  </si>
+  <si>
+    <t>Pickup name</t>
+  </si>
+  <si>
+    <t>Delivery name</t>
+  </si>
+  <si>
+    <t>Order Type</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>florida</t>
+  </si>
+  <si>
+    <t>nevada</t>
+  </si>
+  <si>
+    <t>Inbound Intermodal</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Accessorial Charge</t>
+  </si>
+  <si>
+    <t>Interval value</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test acc charge</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Test description</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Create order</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Customer Reference no.</t>
+  </si>
+  <si>
+    <t>Pickup date and time</t>
+  </si>
+  <si>
+    <t>Delivery date and time</t>
+  </si>
+  <si>
+    <t>Container #</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Container Type</t>
+  </si>
+  <si>
+    <t>Container Owner</t>
+  </si>
+  <si>
+    <t>Order notes</t>
+  </si>
+  <si>
+    <t>Test Customer</t>
+  </si>
+  <si>
+    <t>CONT-111111-1</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>final container</t>
+  </si>
+  <si>
+    <t>final chassis</t>
+  </si>
+  <si>
+    <t>final location</t>
+  </si>
+  <si>
+    <t>CUSTOM567AS</t>
   </si>
 </sst>
 </file>
@@ -211,7 +443,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -226,6 +458,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,22 +804,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
     <col min="2" max="3" width="18.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
     <col min="5" max="6" width="20.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="14" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="11" width="15" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -747,24 +985,384 @@
         <v>46</v>
       </c>
     </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1"/>
     <hyperlink ref="C15" r:id="rId2"/>
+    <hyperlink ref="C19" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>